<commit_message>
UI: roll back on first page
</commit_message>
<xml_diff>
--- a/docs/Output Variable List.xlsx
+++ b/docs/Output Variable List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\idep\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27CC6129-2DB7-4101-92A3-134DCD8E063D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96FC058-92F2-440F-A343-7E50DFA5C0DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5145" windowWidth="29040" windowHeight="15840" xr2:uid="{45A7A2D9-4FF5-4097-8083-5A8E8A30EB10}"/>
+    <workbookView xWindow="46230" yWindow="6540" windowWidth="23040" windowHeight="12210" xr2:uid="{45A7A2D9-4FF5-4097-8083-5A8E8A30EB10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>DataSource</t>
+  </si>
+  <si>
+    <t>Public', 'Client', 'Demo'</t>
+  </si>
+  <si>
+    <t>Store which data source user selected</t>
+  </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>Avaiable Values</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,16 +63,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -57,17 +112,145 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -78,6 +261,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6C9257C2-B5D1-460E-8629-B56E22C1FEF4}" name="Table1" displayName="Table1" ref="A1:C44" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
+  <autoFilter ref="A1:C44" xr:uid="{B2F5807B-D527-4342-8003-0A2D87A9A544}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DB15C687-30CF-40C0-AA92-13B3EE387366}" name="Variable Name"/>
+    <tableColumn id="2" xr3:uid="{B1528F31-6919-4CDA-8EA2-B1366C3D4690}" name="Avaiable Values"/>
+    <tableColumn id="3" xr3:uid="{24A6E9B6-0AE1-4161-88AD-8ACBA6C1B9B9}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,12 +572,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F2239E-9F28-41D4-99DF-9B257EE28458}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>